<commit_message>
yeni dosya sisteminde ilk değişikilik
</commit_message>
<xml_diff>
--- a/deneme excel.xlsx
+++ b/deneme excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22692359a2a982a3/Masaüstü/githubKullanimiDosya/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22692359a2a982a3/Masaüstü/dosya yeni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_AD4D0BC4A776854ACB15BCFDA6D6C462683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0A5942E-364A-4247-8432-37D9CFB96030}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_AD4D0BC4A776854ACB15BCFDA6D6C462683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1359657D-EC30-4BB8-9AF8-2F0CF6961135}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>deneme</t>
+  </si>
+  <si>
+    <t>deneme1</t>
   </si>
 </sst>
 </file>
@@ -345,15 +348,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>